<commit_message>
Added the generation of spreadsheets for the data used to train and test the model
</commit_message>
<xml_diff>
--- a/out/img/core/old/performance_sarima_2023.xlsx
+++ b/out/img/core/old/performance_sarima_2023.xlsx
@@ -689,7 +689,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.804310810063124</v>
+        <v>0.4786985988024913</v>
       </c>
     </row>
     <row r="3">
@@ -699,7 +699,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3.36842651783084</v>
+        <v>1.87279223225016</v>
       </c>
     </row>
   </sheetData>

</xml_diff>